<commit_message>
Double Circular Linked List: Implementation updated. Leetcode: 141, 142 solution added
</commit_message>
<xml_diff>
--- a/Syllabus.xlsx
+++ b/Syllabus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11040" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Java_FSD" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="223">
   <si>
     <t>Topic</t>
   </si>
@@ -875,387 +875,174 @@
     <t>Sub-Topic</t>
   </si>
   <si>
-    <t>Day 1</t>
-  </si>
-  <si>
     <t>Keywords, list, tuple, dictionaries</t>
   </si>
   <si>
-    <t>Day 2</t>
-  </si>
-  <si>
-    <t>Day 3</t>
-  </si>
-  <si>
-    <t>Day 4</t>
-  </si>
-  <si>
-    <t>Day 5</t>
-  </si>
-  <si>
     <t>1D, 2D Arrays, Multi-Dimensional Arrays, Dynamic Arrays (Lists)</t>
   </si>
   <si>
-    <t>Day 6</t>
-  </si>
-  <si>
     <t>Arrays (Hands-on)</t>
   </si>
   <si>
     <t>Array Operations: Insertion, Deletion</t>
   </si>
   <si>
-    <t>Day 7</t>
-  </si>
-  <si>
     <t>Traversal, Searching, Sorting</t>
   </si>
   <si>
-    <t>Day 8</t>
-  </si>
-  <si>
-    <t>Day 9</t>
-  </si>
-  <si>
     <t>Linked Lists (Hands-on)</t>
   </si>
   <si>
     <t>Implementing Singly Linked List (Insert, Delete)</t>
   </si>
   <si>
-    <t>Day 10</t>
-  </si>
-  <si>
     <t>Implementing Singly Linked List (Reverse, Search)</t>
   </si>
   <si>
-    <t>Day 11</t>
-  </si>
-  <si>
-    <t>Day 12</t>
-  </si>
-  <si>
     <t>Doubly &amp; Circular Linked Lists (Hands-on)</t>
   </si>
   <si>
     <t>Implementing Doubly Linked Lists</t>
   </si>
   <si>
-    <t>Day 13</t>
-  </si>
-  <si>
     <t>Implementing Circular Linked Lists</t>
   </si>
   <si>
-    <t>Day 14</t>
-  </si>
-  <si>
-    <t>Day 15</t>
-  </si>
-  <si>
     <t>Stacks (Hands-on)</t>
   </si>
   <si>
-    <t>Implementing Stack Using Arrays</t>
-  </si>
-  <si>
-    <t>Day 16</t>
-  </si>
-  <si>
     <t>Implementing Stack Using Linked Lists</t>
   </si>
   <si>
-    <t>Day 17</t>
-  </si>
-  <si>
-    <t>Day 18</t>
-  </si>
-  <si>
     <t>Queues (Hands-on)</t>
   </si>
   <si>
     <t>Implementing Queue Using Arrays</t>
   </si>
   <si>
-    <t>Day 19</t>
-  </si>
-  <si>
     <t>Implementing Queue Using Linked Lists</t>
   </si>
   <si>
-    <t>Day 20</t>
-  </si>
-  <si>
-    <t>Day 21</t>
-  </si>
-  <si>
     <t>Advanced Queues (Hands-on)</t>
   </si>
   <si>
-    <t>Day 22</t>
-  </si>
-  <si>
-    <t>Day 23</t>
-  </si>
-  <si>
     <t>Recursion in Data Structures (Hands-on)</t>
   </si>
   <si>
     <t>Recursive Algorithms (Factorial, Fibonacci)</t>
   </si>
   <si>
-    <t>Day 24</t>
-  </si>
-  <si>
     <t>Recursive Algorithms (Tree Traversals)</t>
   </si>
   <si>
-    <t>Day 25</t>
-  </si>
-  <si>
-    <t>Day 26</t>
-  </si>
-  <si>
     <t>Trees (Hands-on)</t>
   </si>
   <si>
     <t>Implementing Binary Search Tree (BST)</t>
   </si>
   <si>
-    <t>Day 27</t>
-  </si>
-  <si>
     <t>Tree Traversal Algorithms</t>
   </si>
   <si>
-    <t>Day 28</t>
-  </si>
-  <si>
-    <t>Day 29</t>
-  </si>
-  <si>
     <t>Binary Search Trees (BST) (Hands-on)</t>
   </si>
   <si>
     <t>Implementing BST Operations</t>
   </si>
   <si>
-    <t>Day 30</t>
-  </si>
-  <si>
     <t>AVL Tree Rotation</t>
   </si>
   <si>
-    <t>Day 31</t>
-  </si>
-  <si>
-    <t>Day 32</t>
-  </si>
-  <si>
     <t>Graphs (Hands-on)</t>
   </si>
   <si>
     <t>Implementing Graphs (DFS Traversal)</t>
   </si>
   <si>
-    <t>Day 33</t>
-  </si>
-  <si>
     <t>Implementing Graphs (BFS Traversal)</t>
   </si>
   <si>
-    <t>Day 34</t>
-  </si>
-  <si>
     <t>Concept, Hash Functions</t>
   </si>
   <si>
-    <t>Day 35</t>
-  </si>
-  <si>
-    <t>Day 36</t>
-  </si>
-  <si>
     <t>Hashing (Hands-on)</t>
   </si>
   <si>
     <t>Implementing Hash Tables</t>
   </si>
   <si>
-    <t>Day 37</t>
-  </si>
-  <si>
     <t>Collision Handling</t>
   </si>
   <si>
-    <t>Day 38</t>
-  </si>
-  <si>
     <t>Bubble, Selection, Insertion Sort</t>
   </si>
   <si>
-    <t>Day 39</t>
-  </si>
-  <si>
-    <t>Day 40</t>
-  </si>
-  <si>
     <t>Sorting Algorithms (Hands-on)</t>
   </si>
   <si>
-    <t>Day 41</t>
-  </si>
-  <si>
     <t>Analyzing Time Complexity</t>
   </si>
   <si>
-    <t>Day 42</t>
-  </si>
-  <si>
-    <t>Day 43</t>
-  </si>
-  <si>
     <t>Searching Algorithms (Hands-on)</t>
   </si>
   <si>
     <t>Implementing Search Algorithms</t>
   </si>
   <si>
-    <t>Day 44</t>
-  </si>
-  <si>
     <t>Time Complexity Analysis</t>
   </si>
   <si>
-    <t>Day 45</t>
-  </si>
-  <si>
-    <t>Day 46</t>
-  </si>
-  <si>
     <t>Heaps (Hands-on)</t>
   </si>
   <si>
     <t>Implementing Min Heap</t>
   </si>
   <si>
-    <t>Day 47</t>
-  </si>
-  <si>
     <t>Implementing Max Heap, Heap Sort</t>
   </si>
   <si>
-    <t>Day 48</t>
-  </si>
-  <si>
     <t>Introduction, Approach (Memoization, Tabulation)</t>
   </si>
   <si>
-    <t>Day 49</t>
-  </si>
-  <si>
     <t>Classic DP Problems (Knapsack, LCS)</t>
   </si>
   <si>
-    <t>Day 50</t>
-  </si>
-  <si>
     <t>Dynamic Programming (DP) (Hands-on)</t>
   </si>
   <si>
     <t>Solving DP Problems</t>
   </si>
   <si>
-    <t>Day 51</t>
-  </si>
-  <si>
     <t>Analyzing Space-Time Trade-offs</t>
   </si>
   <si>
-    <t>Day 52</t>
-  </si>
-  <si>
     <t>Concept, Greedy vs. DP</t>
   </si>
   <si>
-    <t>Day 53</t>
-  </si>
-  <si>
     <t>Problems (Activity Selection, Huffman Coding)</t>
   </si>
   <si>
-    <t>Day 54</t>
-  </si>
-  <si>
     <t>Greedy Algorithms (Hands-on)</t>
   </si>
   <si>
     <t>Implementing Greedy Solutions</t>
   </si>
   <si>
-    <t>Day 55</t>
-  </si>
-  <si>
     <t>Analyzing Optimality</t>
   </si>
   <si>
-    <t>Day 56</t>
-  </si>
-  <si>
     <t>Shortest Path Algorithms (Dijkstra, Bellman-Ford)</t>
   </si>
   <si>
-    <t>Day 57</t>
-  </si>
-  <si>
     <t>Minimum Spanning Tree (Kruskal, Prim)</t>
   </si>
   <si>
-    <t>Day 58</t>
-  </si>
-  <si>
     <t>Graph Algorithms (Hands-on)</t>
   </si>
   <si>
     <t>Implementing Graph Algorithms</t>
   </si>
   <si>
-    <t>Day 59</t>
-  </si>
-  <si>
-    <t>Day 60</t>
-  </si>
-  <si>
-    <t>Day 61</t>
-  </si>
-  <si>
-    <t>Day 62</t>
-  </si>
-  <si>
-    <t>Day 63</t>
-  </si>
-  <si>
-    <t>Day 64</t>
-  </si>
-  <si>
-    <t>Day 65</t>
-  </si>
-  <si>
-    <t>Day 66</t>
-  </si>
-  <si>
-    <t>Day 67</t>
-  </si>
-  <si>
-    <t>Day 68</t>
-  </si>
-  <si>
-    <t>Day 69</t>
-  </si>
-  <si>
-    <t>Day 70</t>
-  </si>
-  <si>
     <t>Problem Solving</t>
   </si>
   <si>
@@ -1269,6 +1056,12 @@
   </si>
   <si>
     <t>Functions, Lambda Functions, List comprehension</t>
+  </si>
+  <si>
+    <t>8, 9</t>
+  </si>
+  <si>
+    <t>Assessment</t>
   </si>
 </sst>
 </file>
@@ -1383,7 +1176,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1419,6 +1212,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1639,10 +1442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1767,8 +1570,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <v>8</v>
+      <c r="A9" s="9" t="s">
+        <v>221</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>2</v>
@@ -1783,405 +1586,430 @@
         <v>45668</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="D10" s="8">
+        <v>45677</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>11</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="D11" s="8">
+        <v>45678</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="D12" s="8">
+        <v>45679</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>13</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="D13" s="8">
+        <v>45680</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>14</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="D14" s="8">
+        <v>45681</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>15</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="D15" s="8">
+        <v>45682</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>16</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="D16" s="10">
+        <v>45684</v>
+      </c>
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
+        <v>17</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="D17" s="8">
+        <v>45685</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
+        <v>18</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
+        <v>19</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <v>20</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
+        <v>22</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
+        <v>23</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="16">
+        <v>24</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
+        <v>25</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="16">
+        <v>26</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="16">
+        <v>27</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <v>26</v>
-      </c>
-      <c r="B27" s="4" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="16">
+        <v>28</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <v>27</v>
-      </c>
-      <c r="B28" s="4" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="16">
+        <v>29</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>28</v>
-      </c>
-      <c r="B29" s="4" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="16">
+        <v>30</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>29</v>
-      </c>
-      <c r="B30" s="4" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="16">
+        <v>31</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>30</v>
-      </c>
-      <c r="B31" s="4" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="16">
+        <v>32</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <v>31</v>
-      </c>
-      <c r="B32" s="4" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="16">
+        <v>33</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <v>32</v>
-      </c>
-      <c r="B33" s="4" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="16">
+        <v>34</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <v>33</v>
-      </c>
-      <c r="B34" s="4" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="16">
+        <v>35</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
-        <v>34</v>
-      </c>
-      <c r="B35" s="4" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="16">
+        <v>36</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <v>35</v>
-      </c>
-      <c r="B36" s="4" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="16">
+        <v>37</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <v>36</v>
-      </c>
-      <c r="B37" s="4" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="16">
+        <v>38</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
-        <v>37</v>
-      </c>
-      <c r="B38" s="4" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="16">
+        <v>39</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
-        <v>38</v>
-      </c>
-      <c r="B39" s="4" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="16">
+        <v>40</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
-        <v>39</v>
-      </c>
-      <c r="B40" s="4" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="16">
+        <v>41</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
-        <v>40</v>
-      </c>
-      <c r="B41" s="4" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="16">
+        <v>42</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
-        <v>41</v>
-      </c>
-      <c r="B42" s="4" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="16">
+        <v>43</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
-        <v>42</v>
-      </c>
-      <c r="B43" s="4" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="16">
+        <v>44</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
-        <v>43</v>
-      </c>
-      <c r="B44" s="4" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="16">
+        <v>45</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
-        <v>44</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
-        <v>45</v>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="16">
+        <v>46</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>83</v>
@@ -2190,75 +2018,75 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
-        <v>46</v>
-      </c>
-      <c r="B47" s="4" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="16">
+        <v>47</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="16">
+        <v>48</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
-        <v>47</v>
-      </c>
-      <c r="B48" s="4" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="16">
+        <v>49</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C49" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
-        <v>48</v>
-      </c>
-      <c r="B49" s="4" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="16">
+        <v>50</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
-        <v>49</v>
-      </c>
-      <c r="B50" s="4" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="16">
+        <v>51</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
-        <v>50</v>
-      </c>
-      <c r="B51" s="4" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="16">
+        <v>52</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
-        <v>52</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="2">
-        <v>52</v>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="16">
+        <v>53</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>7</v>
@@ -2267,9 +2095,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="2">
-        <v>53</v>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="16">
+        <v>54</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>7</v>
@@ -2278,9 +2106,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
-        <v>54</v>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="16">
+        <v>55</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>7</v>
@@ -2289,179 +2117,190 @@
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="2">
-        <v>55</v>
-      </c>
-      <c r="B56" s="4" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="16">
+        <v>56</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="16">
+        <v>57</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C57" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="2">
-        <v>56</v>
-      </c>
-      <c r="B57" s="4" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="16">
+        <v>58</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C58" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="2">
-        <v>57</v>
-      </c>
-      <c r="B58" s="4" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="16">
+        <v>59</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C59" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="2">
-        <v>58</v>
-      </c>
-      <c r="B59" s="4" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="16">
+        <v>60</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C60" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="2">
-        <v>59</v>
-      </c>
-      <c r="B60" s="4" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="16">
+        <v>61</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C61" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="2">
-        <v>60</v>
-      </c>
-      <c r="B61" s="4" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="16">
+        <v>62</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C62" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="2">
-        <v>61</v>
-      </c>
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A63" s="16">
+        <v>63</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C63" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="2">
-        <v>62</v>
-      </c>
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A64" s="16">
+        <v>64</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C64" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A64" s="2">
-        <v>63</v>
-      </c>
-      <c r="B64" s="4" t="s">
+    <row r="65" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A65" s="16">
+        <v>65</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C65" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A65" s="2">
-        <v>64</v>
-      </c>
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A66" s="16">
+        <v>66</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C66" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="2">
-        <v>65</v>
-      </c>
-      <c r="B66" s="4" t="s">
+    <row r="67" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A67" s="16">
+        <v>67</v>
+      </c>
+      <c r="B67" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="2">
-        <v>66</v>
-      </c>
-      <c r="B67" s="4" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="16">
+        <v>68</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C68" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="2">
-        <v>67</v>
-      </c>
-      <c r="B68" s="4" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="16">
+        <v>69</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C69" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="2">
-        <v>68</v>
-      </c>
-      <c r="B69" s="4" t="s">
+    <row r="70" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A70" s="16">
+        <v>70</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="2">
-        <v>69</v>
-      </c>
-      <c r="B70" s="4" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="16">
+        <v>71</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C71" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="2">
-        <v>70</v>
-      </c>
-      <c r="B71" s="4" t="s">
+    <row r="72" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A72" s="16">
+        <v>72</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C72" s="4" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2475,8 +2314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2503,50 +2342,50 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>160</v>
+      <c r="A2" s="15">
+        <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D2" s="8">
         <v>45659</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>162</v>
+      <c r="A3" s="15">
+        <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>291</v>
+        <v>220</v>
       </c>
       <c r="D3" s="8">
         <v>45660</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>163</v>
+      <c r="A4" s="15">
+        <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>290</v>
+        <v>219</v>
       </c>
       <c r="D4" s="8">
         <v>45661</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>164</v>
+      <c r="A5" s="15">
+        <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>9</v>
@@ -2559,8 +2398,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>165</v>
+      <c r="A6" s="15">
+        <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>9</v>
@@ -2573,108 +2412,120 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>167</v>
+      <c r="A7" s="15">
+        <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>289</v>
+        <v>218</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>287</v>
+        <v>216</v>
       </c>
       <c r="D7" s="8">
         <v>45665</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>170</v>
+      <c r="A8" s="15">
+        <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D8" s="8">
         <v>45666</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>172</v>
+      <c r="A9" s="15">
+        <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D9" s="8">
         <v>45667</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>173</v>
+      <c r="A10" s="15">
+        <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D10" s="8">
         <v>45668</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>10</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>287</v>
+      <c r="D11" s="8">
+        <v>45677</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>11</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" s="8">
+        <v>45678</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>12</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="8">
+        <v>45679</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>13</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D14" s="8">
+        <v>45680</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
-        <v>184</v>
+      <c r="A15" s="16">
+        <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>15</v>
@@ -2682,65 +2533,77 @@
       <c r="C15" s="12" t="s">
         <v>16</v>
       </c>
+      <c r="D15" s="8">
+        <v>45681</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
-        <v>185</v>
+      <c r="A16" s="16">
+        <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
-        <v>188</v>
+        <v>169</v>
+      </c>
+      <c r="D16" s="8">
+        <v>45682</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>180</v>
+        <v>222</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
-        <v>190</v>
+        <v>222</v>
+      </c>
+      <c r="D17" s="8">
+        <v>45684</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="16">
+        <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" s="8">
+        <v>45685</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
+        <v>18</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C19" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>194</v>
+    <row r="20" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="16">
+        <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
-        <v>196</v>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="16">
+        <v>20</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>19</v>
@@ -2749,31 +2612,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>197</v>
+    <row r="22" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="16">
+        <v>21</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
-        <v>199</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="16">
+        <v>22</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
-        <v>200</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="16">
+        <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>21</v>
@@ -2782,31 +2645,31 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
-        <v>203</v>
+    <row r="25" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="16">
+        <v>24</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
-        <v>205</v>
+    <row r="26" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="16">
+        <v>25</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
-        <v>206</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="16">
+        <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>24</v>
@@ -2815,31 +2678,31 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
-        <v>209</v>
+    <row r="28" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="16">
+        <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
-        <v>211</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="16">
+        <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
-        <v>212</v>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="16">
+        <v>29</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>26</v>
@@ -2848,42 +2711,42 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
-        <v>215</v>
+    <row r="31" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="16">
+        <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="12" t="s">
-        <v>217</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="16">
+        <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="12" t="s">
-        <v>218</v>
+      <c r="A33" s="16">
+        <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>287</v>
+        <v>216</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="12" t="s">
-        <v>221</v>
+      <c r="A34" s="16">
+        <v>33</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>28</v>
@@ -2893,30 +2756,30 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="s">
-        <v>223</v>
+      <c r="A35" s="16">
+        <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
-        <v>225</v>
+      <c r="A36" s="16">
+        <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>216</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="12" t="s">
-        <v>226</v>
+      <c r="A37" s="16">
+        <v>36</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>30</v>
@@ -2926,52 +2789,52 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="12" t="s">
-        <v>229</v>
+      <c r="A38" s="16">
+        <v>37</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>219</v>
+        <v>186</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A39" s="12" t="s">
-        <v>231</v>
+      <c r="A39" s="16">
+        <v>38</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>219</v>
+        <v>186</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>222</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="12" t="s">
-        <v>233</v>
+      <c r="A40" s="16">
+        <v>39</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>219</v>
+        <v>186</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>287</v>
+        <v>216</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="12" t="s">
-        <v>234</v>
+      <c r="A41" s="16">
+        <v>40</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>32</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="12" t="s">
-        <v>236</v>
+      <c r="A42" s="16">
+        <v>41</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>32</v>
@@ -2981,129 +2844,129 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A43" s="12" t="s">
-        <v>238</v>
+      <c r="A43" s="16">
+        <v>42</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>228</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="12" t="s">
-        <v>239</v>
+      <c r="A44" s="16">
+        <v>43</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>230</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="12" t="s">
-        <v>242</v>
+      <c r="A45" s="16">
+        <v>44</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>33</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>232</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="12" t="s">
-        <v>244</v>
+      <c r="A46" s="16">
+        <v>45</v>
       </c>
       <c r="B46" s="12" t="s">
         <v>33</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>288</v>
+        <v>217</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="12" t="s">
-        <v>245</v>
+      <c r="A47" s="16">
+        <v>46</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>235</v>
+        <v>194</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="12" t="s">
-        <v>248</v>
+      <c r="A48" s="16">
+        <v>47</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>235</v>
+        <v>194</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>237</v>
+        <v>195</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="12" t="s">
-        <v>250</v>
+      <c r="A49" s="16">
+        <v>48</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>235</v>
+        <v>194</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>287</v>
+        <v>216</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="12" t="s">
-        <v>252</v>
+      <c r="A50" s="16">
+        <v>49</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>235</v>
+        <v>194</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>287</v>
+        <v>216</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A51" s="12" t="s">
-        <v>254</v>
+      <c r="A51" s="16">
+        <v>50</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>235</v>
+        <v>194</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>287</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A52" s="12" t="s">
-        <v>257</v>
+      <c r="A52" s="16">
+        <v>51</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>240</v>
+        <v>196</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>241</v>
+        <v>197</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A53" s="12" t="s">
-        <v>259</v>
+      <c r="A53" s="16">
+        <v>52</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>240</v>
+        <v>196</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>243</v>
+        <v>198</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A54" s="12" t="s">
-        <v>261</v>
+      <c r="A54" s="16">
+        <v>53</v>
       </c>
       <c r="B54" s="12" t="s">
         <v>34</v>
@@ -3113,190 +2976,190 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A55" s="12" t="s">
-        <v>263</v>
+      <c r="A55" s="16">
+        <v>54</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>246</v>
+        <v>199</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>247</v>
+        <v>200</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A56" s="12" t="s">
-        <v>266</v>
+      <c r="A56" s="16">
+        <v>55</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>246</v>
+        <v>199</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A57" s="12" t="s">
-        <v>268</v>
+      <c r="A57" s="16">
+        <v>56</v>
       </c>
       <c r="B57" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>287</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A58" s="12" t="s">
-        <v>270</v>
+      <c r="A58" s="16">
+        <v>57</v>
       </c>
       <c r="B58" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>251</v>
+        <v>202</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A59" s="12" t="s">
-        <v>272</v>
+      <c r="A59" s="16">
+        <v>58</v>
       </c>
       <c r="B59" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>253</v>
+        <v>203</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A60" s="12" t="s">
-        <v>275</v>
+      <c r="A60" s="16">
+        <v>59</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>255</v>
+        <v>204</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>256</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A61" s="12" t="s">
-        <v>276</v>
+      <c r="A61" s="16">
+        <v>60</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>255</v>
+        <v>204</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>258</v>
+        <v>206</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A62" s="12" t="s">
-        <v>277</v>
+      <c r="A62" s="16">
+        <v>61</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>255</v>
+        <v>204</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>287</v>
+        <v>216</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A63" s="12" t="s">
-        <v>278</v>
+      <c r="A63" s="16">
+        <v>62</v>
       </c>
       <c r="B63" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>260</v>
+        <v>207</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A64" s="12" t="s">
-        <v>279</v>
+      <c r="A64" s="16">
+        <v>63</v>
       </c>
       <c r="B64" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>262</v>
+        <v>208</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A65" s="12" t="s">
-        <v>280</v>
+      <c r="A65" s="16">
+        <v>64</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>264</v>
+        <v>209</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>265</v>
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A66" s="12" t="s">
-        <v>281</v>
+      <c r="A66" s="16">
+        <v>65</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>264</v>
+        <v>209</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>267</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A67" s="12" t="s">
-        <v>282</v>
+      <c r="A67" s="16">
+        <v>66</v>
       </c>
       <c r="B67" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>269</v>
+        <v>212</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A68" s="12" t="s">
-        <v>283</v>
+      <c r="A68" s="16">
+        <v>67</v>
       </c>
       <c r="B68" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>271</v>
+        <v>213</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A69" s="12" t="s">
-        <v>284</v>
+      <c r="A69" s="16">
+        <v>68</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>273</v>
+        <v>214</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>274</v>
+        <v>215</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A70" s="12" t="s">
-        <v>285</v>
+      <c r="A70" s="16">
+        <v>69</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>273</v>
+        <v>214</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>237</v>
+        <v>195</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A71" s="12" t="s">
-        <v>286</v>
+      <c r="A71" s="16">
+        <v>70</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>273</v>
+        <v>214</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>287</v>
+        <v>216</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Queue: Array and LinkedList implementation added. Leetcode: 1944 solution added
</commit_message>
<xml_diff>
--- a/Syllabus.xlsx
+++ b/Syllabus.xlsx
@@ -1176,7 +1176,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1222,6 +1222,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1444,9 +1445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1686,13 +1685,13 @@
       <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
+      <c r="A17" s="15">
         <v>17</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="17" t="s">
         <v>57</v>
       </c>
       <c r="D17" s="8">
@@ -1700,36 +1699,45 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
+      <c r="A18" s="15">
         <v>18</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="17" t="s">
         <v>59</v>
       </c>
+      <c r="D18" s="8">
+        <v>45686</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="16">
+      <c r="A19" s="15">
         <v>19</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="17" t="s">
         <v>61</v>
       </c>
+      <c r="D19" s="8">
+        <v>45687</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
+      <c r="A20" s="15">
         <v>20</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="17" t="s">
         <v>63</v>
+      </c>
+      <c r="D20" s="8">
+        <v>45688</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2314,9 +2322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
-    </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2523,93 +2529,102 @@
         <v>45680</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="16">
+    <row r="15" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
         <v>14</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="8">
         <v>45681</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="16">
+    <row r="16" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
         <v>15</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="14" t="s">
         <v>169</v>
       </c>
       <c r="D16" s="8">
         <v>45682</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="16">
+    <row r="17" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
         <v>16</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="10">
         <v>45684</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="16">
+    <row r="18" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
         <v>17</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="14" t="s">
         <v>170</v>
       </c>
       <c r="D18" s="8">
         <v>45685</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="16">
+    <row r="19" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="16">
+      <c r="D19" s="8">
+        <v>45686</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
         <v>19</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="14" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="16">
+      <c r="D20" s="8">
+        <v>45687</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
         <v>20</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="19" t="s">
         <v>20</v>
+      </c>
+      <c r="D21" s="8">
+        <v>45688</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
leetcode: 46, 77, 78 solutions are added
</commit_message>
<xml_diff>
--- a/Syllabus.xlsx
+++ b/Syllabus.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ByteXL\MRU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ByteXL\MRU\Java_FSD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Java_FSD" sheetId="3" r:id="rId1"/>
@@ -451,8 +451,14 @@
     <t>Test Coverage, Writing Clean Tests, Debugging Failing Tests, Continuous Testing with CI/CD</t>
   </si>
   <si>
-    <r>
-      <t>Using useState</t>
+    <t>Introduction and Usage of useEffect</t>
+  </si>
+  <si>
+    <t>Creating Custom Hooks, React Memo, and React.memo</t>
+  </si>
+  <si>
+    <r>
+      <t>Using @RestController</t>
     </r>
     <r>
       <rPr>
@@ -461,12 +467,21 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> Hook for Managing State</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>useEffect</t>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>@RequestMapping</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Using @ControllerAdvice</t>
     </r>
     <r>
       <rPr>
@@ -475,15 +490,21 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> Hook</t>
-    </r>
-  </si>
-  <si>
-    <t>Introduction and Usage of useEffect</t>
-  </si>
-  <si>
-    <r>
-      <t>Route Parameters, Using useParams</t>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>@ExceptionHandler</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Creating APIs, @RestController</t>
     </r>
     <r>
       <rPr>
@@ -492,7 +513,21 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> and </t>
+      <t>, Spring Boot DevTools</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Query Operators ($and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
     </r>
     <r>
       <rPr>
@@ -501,15 +536,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>useNavigate</t>
-    </r>
-  </si>
-  <si>
-    <t>Creating Custom Hooks, React Memo, and React.memo</t>
-  </si>
-  <si>
-    <r>
-      <t>Using @RestController</t>
+      <t>$or</t>
     </r>
     <r>
       <rPr>
@@ -527,12 +554,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>@RequestMapping</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Using @ControllerAdvice</t>
+      <t>$gt</t>
     </r>
     <r>
       <rPr>
@@ -541,7 +563,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> and </t>
+      <t xml:space="preserve">, </t>
     </r>
     <r>
       <rPr>
@@ -550,12 +572,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>@ExceptionHandler</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Creating APIs, @RestController</t>
+      <t>$lt</t>
     </r>
     <r>
       <rPr>
@@ -564,12 +581,16 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>, Spring Boot DevTools</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Query Operators ($and</t>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>$in</t>
     </r>
     <r>
       <rPr>
@@ -578,6 +599,20 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
+      <t>), Regular Expressions, and Text Search</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Aggregation Pipeline, $match</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">, </t>
     </r>
     <r>
@@ -587,7 +622,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>$or</t>
+      <t>$group</t>
     </r>
     <r>
       <rPr>
@@ -605,7 +640,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>$gt</t>
+      <t>$project</t>
     </r>
     <r>
       <rPr>
@@ -614,6 +649,20 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
+      <t>, Sorting, and Limiting</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Writing First Test, Test Lifecycle (@Before</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">, </t>
     </r>
     <r>
@@ -623,7 +672,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>$lt</t>
+      <t>@After</t>
     </r>
     <r>
       <rPr>
@@ -641,7 +690,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>$in</t>
+      <t>@BeforeClass</t>
     </r>
     <r>
       <rPr>
@@ -650,12 +699,16 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>), Regular Expressions, and Text Search</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Aggregation Pipeline, $match</t>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>@AfterClass</t>
     </r>
     <r>
       <rPr>
@@ -664,6 +717,20 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
+      <t>), Assertions</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Assertions (assertEquals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">, </t>
     </r>
     <r>
@@ -673,7 +740,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>$group</t>
+      <t>assertNotNull</t>
     </r>
     <r>
       <rPr>
@@ -691,7 +758,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>$project</t>
+      <t>assertThrows</t>
     </r>
     <r>
       <rPr>
@@ -700,12 +767,12 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>, Sorting, and Limiting</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Writing First Test, Test Lifecycle (@Before</t>
+      <t>), Test Suites, Parameterized Tests</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Spring Testing Annotations (@RunWith</t>
     </r>
     <r>
       <rPr>
@@ -723,7 +790,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>@After</t>
+      <t>@SpringBootTest</t>
     </r>
     <r>
       <rPr>
@@ -732,7 +799,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">, </t>
+      <t xml:space="preserve">), Mocking Beans with </t>
     </r>
     <r>
       <rPr>
@@ -741,124 +808,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>@BeforeClass</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>@AfterClass</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>), Assertions</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Assertions (assertEquals</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>assertNotNull</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>assertThrows</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>), Test Suites, Parameterized Tests</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Spring Testing Annotations (@RunWith</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>@SpringBootTest</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">), Mocking Beans with </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>@MockBean</t>
     </r>
   </si>
@@ -1062,6 +1011,15 @@
   </si>
   <si>
     <t>Assessment</t>
+  </si>
+  <si>
+    <t>Using useState Hook for Managing State</t>
+  </si>
+  <si>
+    <t>useEffect Hook</t>
+  </si>
+  <si>
+    <t>Route Parameters, Using useParams and useNavigate</t>
   </si>
 </sst>
 </file>
@@ -1445,14 +1403,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.5546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="73.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
@@ -1467,7 +1428,7 @@
         <v>40</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1570,7 +1531,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>2</v>
@@ -1674,10 +1635,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D16" s="10">
         <v>45684</v>
@@ -1741,80 +1702,101 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
+      <c r="A21" s="15">
         <v>21</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="17" t="s">
         <v>65</v>
       </c>
+      <c r="D21" s="8">
+        <v>45689</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="16">
+      <c r="A22" s="15">
         <v>22</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="D22" s="8">
+        <v>45691</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <v>23</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="8">
+        <v>45692</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>24</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="16">
-        <v>23</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="16">
-        <v>24</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>145</v>
+      <c r="D24" s="8">
+        <v>45693</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="16">
+      <c r="A25" s="15">
         <v>25</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="17" t="s">
         <v>70</v>
       </c>
+      <c r="D25" s="8">
+        <v>45694</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="16">
+      <c r="A26" s="15">
         <v>26</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>146</v>
+      <c r="C26" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="D26" s="8">
+        <v>45695</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="16">
+      <c r="A27" s="15">
         <v>27</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="17" t="s">
         <v>73</v>
+      </c>
+      <c r="D27" s="8">
+        <v>45696</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1827,6 +1809,9 @@
       <c r="C28" s="4" t="s">
         <v>75</v>
       </c>
+      <c r="D28" s="8">
+        <v>45698</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
@@ -1869,7 +1854,7 @@
         <v>82</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1990,7 +1975,7 @@
         <v>102</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2012,7 +1997,7 @@
         <v>105</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2056,7 +2041,7 @@
         <v>109</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2188,7 +2173,7 @@
         <v>124</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -2199,7 +2184,7 @@
         <v>125</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
@@ -2254,7 +2239,7 @@
         <v>134</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2265,7 +2250,7 @@
         <v>135</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2287,7 +2272,7 @@
         <v>138</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2322,14 +2307,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.88671875" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.109375" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
@@ -2341,10 +2328,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
@@ -2355,7 +2342,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D2" s="8">
         <v>45659</v>
@@ -2369,7 +2356,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D3" s="8">
         <v>45660</v>
@@ -2383,7 +2370,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D4" s="8">
         <v>45661</v>
@@ -2422,10 +2409,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D7" s="8">
         <v>45665</v>
@@ -2439,7 +2426,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D8" s="8">
         <v>45666</v>
@@ -2450,10 +2437,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D9" s="8">
         <v>45667</v>
@@ -2464,10 +2451,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D10" s="8">
         <v>45668</v>
@@ -2492,10 +2479,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D12" s="8">
         <v>45678</v>
@@ -2506,10 +2493,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D13" s="8">
         <v>45679</v>
@@ -2520,10 +2507,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D14" s="8">
         <v>45680</v>
@@ -2548,10 +2535,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D16" s="8">
         <v>45682</v>
@@ -2562,10 +2549,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D17" s="10">
         <v>45684</v>
@@ -2576,10 +2563,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D18" s="8">
         <v>45685</v>
@@ -2604,10 +2591,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D20" s="8">
         <v>45687</v>
@@ -2627,81 +2614,102 @@
         <v>45688</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="16">
+    <row r="22" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
         <v>21</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="8">
+        <v>45689</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <v>22</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" s="8">
+        <v>45691</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>23</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="8">
+        <v>45692</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
+        <v>24</v>
+      </c>
+      <c r="B25" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C25" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="8">
+        <v>45693</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <v>25</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="D26" s="8">
+        <v>45694</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <v>26</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="8">
+        <v>45695</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>27</v>
+      </c>
+      <c r="B28" s="14" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="16">
-        <v>22</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C23" s="12" t="s">
+      <c r="C28" s="14" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="16">
-        <v>23</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="16">
-        <v>24</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="16">
-        <v>25</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="16">
-        <v>26</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="16">
-        <v>27</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>178</v>
+      <c r="D28" s="8">
+        <v>45696</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
@@ -2709,10 +2717,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
+      </c>
+      <c r="D29" s="8">
+        <v>45698</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
@@ -2731,10 +2742,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
@@ -2742,10 +2753,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2756,7 +2767,7 @@
         <v>26</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2775,10 +2786,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2786,10 +2797,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2808,10 +2819,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2819,10 +2830,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2830,10 +2841,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2844,7 +2855,7 @@
         <v>32</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2855,7 +2866,7 @@
         <v>32</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2863,10 +2874,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2874,10 +2885,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2888,7 +2899,7 @@
         <v>33</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2899,7 +2910,7 @@
         <v>33</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2907,10 +2918,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2918,10 +2929,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2929,10 +2940,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2940,10 +2951,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2951,10 +2962,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2962,10 +2973,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2973,10 +2984,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2995,10 +3006,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3006,10 +3017,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3020,7 +3031,7 @@
         <v>34</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3031,7 +3042,7 @@
         <v>36</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3042,7 +3053,7 @@
         <v>36</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3050,10 +3061,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3061,10 +3072,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3072,10 +3083,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3086,7 +3097,7 @@
         <v>37</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3097,7 +3108,7 @@
         <v>37</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3105,10 +3116,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3116,10 +3127,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3130,7 +3141,7 @@
         <v>38</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3141,7 +3152,7 @@
         <v>38</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3149,10 +3160,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3160,10 +3171,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3171,10 +3182,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Complete Binary Search Tree Implementation
</commit_message>
<xml_diff>
--- a/Syllabus.xlsx
+++ b/Syllabus.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ByteXL\MRU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ByteXL\MRU\Python_DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1134,7 +1134,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1181,6 +1181,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1404,7 +1411,7 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:D29"/>
+      <selection activeCell="A31" sqref="A31:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1828,50 +1835,62 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="16">
+      <c r="A30" s="15">
         <v>30</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="17" t="s">
         <v>79</v>
       </c>
+      <c r="D30" s="8">
+        <v>45700</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="16">
+      <c r="A31" s="20">
         <v>31</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="22" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="16">
+      <c r="D31" s="8">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A32" s="20">
         <v>32</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="22" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="16">
+      <c r="D32" s="8">
+        <v>45702</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="20">
         <v>33</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="22" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="8">
+        <v>45703</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>34</v>
       </c>
@@ -1882,7 +1901,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
         <v>35</v>
       </c>
@@ -1893,7 +1912,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="16">
         <v>36</v>
       </c>
@@ -1904,7 +1923,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <v>37</v>
       </c>
@@ -1915,7 +1934,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
         <v>38</v>
       </c>
@@ -1926,7 +1945,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="16">
         <v>39</v>
       </c>
@@ -1937,7 +1956,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
         <v>40</v>
       </c>
@@ -1948,7 +1967,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
         <v>41</v>
       </c>
@@ -1959,7 +1978,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
         <v>42</v>
       </c>
@@ -1970,7 +1989,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
         <v>43</v>
       </c>
@@ -1981,7 +2000,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
         <v>44</v>
       </c>
@@ -1992,7 +2011,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
         <v>45</v>
       </c>
@@ -2003,7 +2022,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
         <v>46</v>
       </c>
@@ -2014,7 +2033,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
         <v>47</v>
       </c>
@@ -2025,7 +2044,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
         <v>48</v>
       </c>
@@ -2311,7 +2330,7 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="A32" sqref="A32:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2743,51 +2762,63 @@
         <v>45699</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="16">
+    <row r="31" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
         <v>30</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="14" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="16">
+      <c r="D31" s="8">
+        <v>45700</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A32" s="20">
         <v>31</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="21" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="16">
+      <c r="D32" s="8">
+        <v>45701</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A33" s="20">
         <v>32</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="21" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="16">
+      <c r="D33" s="8">
+        <v>45702</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A34" s="20">
         <v>33</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="21" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D34" s="8">
+        <v>45703</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="16">
         <v>34</v>
       </c>
@@ -2798,7 +2829,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="16">
         <v>35</v>
       </c>
@@ -2809,7 +2840,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="16">
         <v>36</v>
       </c>
@@ -2820,7 +2851,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="16">
         <v>37</v>
       </c>
@@ -2831,7 +2862,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="16">
         <v>38</v>
       </c>
@@ -2842,7 +2873,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="16">
         <v>39</v>
       </c>
@@ -2853,7 +2884,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="16">
         <v>40</v>
       </c>
@@ -2864,7 +2895,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="16">
         <v>41</v>
       </c>
@@ -2875,7 +2906,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" s="16">
         <v>42</v>
       </c>
@@ -2886,7 +2917,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="16">
         <v>43</v>
       </c>
@@ -2897,7 +2928,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="16">
         <v>44</v>
       </c>
@@ -2908,7 +2939,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" s="16">
         <v>45</v>
       </c>
@@ -2919,7 +2950,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" s="16">
         <v>46</v>
       </c>
@@ -2930,7 +2961,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" s="16">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
leetcode: 560 solution added
</commit_message>
<xml_diff>
--- a/Syllabus.xlsx
+++ b/Syllabus.xlsx
@@ -1410,7 +1410,7 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2002,13 +2002,13 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="16">
+      <c r="A42" s="15">
         <v>42</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="17" t="s">
         <v>101</v>
       </c>
       <c r="D42" s="8">
@@ -2024,6 +2024,9 @@
       </c>
       <c r="C43" s="4" t="s">
         <v>145</v>
+      </c>
+      <c r="D43" s="8">
+        <v>45720</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2356,7 +2359,7 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2956,14 +2959,14 @@
         <v>45717</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A43" s="16">
+    <row r="43" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A43" s="15">
         <v>42</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" s="14" t="s">
         <v>188</v>
       </c>
       <c r="D43" s="8">
@@ -2979,6 +2982,9 @@
       </c>
       <c r="C44" s="12" t="s">
         <v>189</v>
+      </c>
+      <c r="D44" s="8">
+        <v>45720</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Leetcode: 2251, 2551 solution added.
</commit_message>
<xml_diff>
--- a/Syllabus.xlsx
+++ b/Syllabus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11040" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Java_FSD" sheetId="3" r:id="rId1"/>
@@ -458,7 +458,21 @@
   </si>
   <si>
     <r>
-      <t>Using @RestController</t>
+      <t>Creating APIs, @RestController</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, Spring Boot DevTools</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Query Operators ($and</t>
     </r>
     <r>
       <rPr>
@@ -476,49 +490,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>@RequestMapping</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Using @ControllerAdvice</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>@ExceptionHandler</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Creating APIs, @RestController</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, Spring Boot DevTools</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Query Operators ($and</t>
+      <t>$or</t>
     </r>
     <r>
       <rPr>
@@ -536,7 +508,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>$or</t>
+      <t>$gt</t>
     </r>
     <r>
       <rPr>
@@ -554,7 +526,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>$gt</t>
+      <t>$lt</t>
     </r>
     <r>
       <rPr>
@@ -572,7 +544,21 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>$lt</t>
+      <t>$in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>), Regular Expressions, and Text Search</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Aggregation Pipeline, $match</t>
     </r>
     <r>
       <rPr>
@@ -590,21 +576,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>$in</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>), Regular Expressions, and Text Search</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Aggregation Pipeline, $match</t>
+      <t>$group</t>
     </r>
     <r>
       <rPr>
@@ -622,7 +594,21 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>$group</t>
+      <t>$project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, Sorting, and Limiting</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Writing First Test, Test Lifecycle (@Before</t>
     </r>
     <r>
       <rPr>
@@ -640,21 +626,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>$project</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, Sorting, and Limiting</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Writing First Test, Test Lifecycle (@Before</t>
+      <t>@After</t>
     </r>
     <r>
       <rPr>
@@ -672,7 +644,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>@After</t>
+      <t>@BeforeClass</t>
     </r>
     <r>
       <rPr>
@@ -690,7 +662,21 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>@BeforeClass</t>
+      <t>@AfterClass</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>), Assertions</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Assertions (assertEquals</t>
     </r>
     <r>
       <rPr>
@@ -708,21 +694,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>@AfterClass</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>), Assertions</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Assertions (assertEquals</t>
+      <t>assertNotNull</t>
     </r>
     <r>
       <rPr>
@@ -740,7 +712,21 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>assertNotNull</t>
+      <t>assertThrows</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>), Test Suites, Parameterized Tests</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Spring Testing Annotations (@RunWith</t>
     </r>
     <r>
       <rPr>
@@ -758,38 +744,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>assertThrows</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>), Test Suites, Parameterized Tests</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Spring Testing Annotations (@RunWith</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>@SpringBootTest</t>
     </r>
     <r>
@@ -1020,6 +974,12 @@
   </si>
   <si>
     <t>Route Parameters, Using useParams and useNavigate</t>
+  </si>
+  <si>
+    <t>Using @RestController, @RequestMapping</t>
+  </si>
+  <si>
+    <t>Using @ControllerAdvice and @ExceptionHandler</t>
   </si>
 </sst>
 </file>
@@ -1409,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1434,7 +1394,7 @@
         <v>40</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1537,7 +1497,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>2</v>
@@ -1641,10 +1601,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D16" s="10">
         <v>45684</v>
@@ -1729,7 +1689,7 @@
         <v>66</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D22" s="8">
         <v>45691</v>
@@ -1754,7 +1714,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>143</v>
@@ -1785,7 +1745,7 @@
         <v>71</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D26" s="8">
         <v>45695</v>
@@ -2016,39 +1976,45 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="16">
+      <c r="A43" s="15">
         <v>43</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>145</v>
+      <c r="C43" s="17" t="s">
+        <v>221</v>
       </c>
       <c r="D43" s="8">
         <v>45720</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="16">
+      <c r="A44" s="15">
         <v>44</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="17" t="s">
         <v>104</v>
       </c>
+      <c r="D44" s="8">
+        <v>45721</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="16">
+      <c r="A45" s="15">
         <v>45</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>146</v>
+      <c r="C45" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="D45" s="8">
+        <v>45722</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2061,6 +2027,9 @@
       <c r="C46" s="3" t="s">
         <v>106</v>
       </c>
+      <c r="D46" s="8">
+        <v>45723</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
@@ -2092,7 +2061,7 @@
         <v>109</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2224,7 +2193,7 @@
         <v>124</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -2235,7 +2204,7 @@
         <v>125</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
@@ -2290,7 +2259,7 @@
         <v>134</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2301,7 +2270,7 @@
         <v>135</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2323,7 +2292,7 @@
         <v>138</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2358,8 +2327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46:D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2379,10 +2348,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
@@ -2393,7 +2362,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D2" s="8">
         <v>45659</v>
@@ -2407,7 +2376,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D3" s="8">
         <v>45660</v>
@@ -2421,7 +2390,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D4" s="8">
         <v>45661</v>
@@ -2460,10 +2429,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D7" s="8">
         <v>45665</v>
@@ -2477,7 +2446,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D8" s="8">
         <v>45666</v>
@@ -2488,10 +2457,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D9" s="8">
         <v>45667</v>
@@ -2502,10 +2471,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>159</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>161</v>
       </c>
       <c r="D10" s="8">
         <v>45668</v>
@@ -2530,10 +2499,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D12" s="8">
         <v>45678</v>
@@ -2544,10 +2513,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>162</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>164</v>
       </c>
       <c r="D13" s="8">
         <v>45679</v>
@@ -2558,10 +2527,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D14" s="8">
         <v>45680</v>
@@ -2586,10 +2555,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D16" s="8">
         <v>45682</v>
@@ -2600,10 +2569,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D17" s="10">
         <v>45684</v>
@@ -2614,10 +2583,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>165</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>167</v>
       </c>
       <c r="D18" s="8">
         <v>45685</v>
@@ -2642,10 +2611,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D20" s="8">
         <v>45687</v>
@@ -2670,10 +2639,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D22" s="8">
         <v>45689</v>
@@ -2684,10 +2653,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>170</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>172</v>
       </c>
       <c r="D23" s="8">
         <v>45691</v>
@@ -2712,7 +2681,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>23</v>
@@ -2726,10 +2695,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D26" s="8">
         <v>45694</v>
@@ -2754,10 +2723,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D28" s="8">
         <v>45696</v>
@@ -2768,10 +2737,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>174</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>176</v>
       </c>
       <c r="D29" s="8">
         <v>45698</v>
@@ -2796,10 +2765,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D31" s="8">
         <v>45700</v>
@@ -2810,10 +2779,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>177</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>179</v>
       </c>
       <c r="D32" s="8">
         <v>45701</v>
@@ -2827,7 +2796,7 @@
         <v>26</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D33" s="8">
         <v>45702</v>
@@ -2852,10 +2821,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D35" s="8">
         <v>45705</v>
@@ -2866,10 +2835,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C36" s="14" t="s">
         <v>180</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>182</v>
       </c>
       <c r="D36" s="8">
         <v>45706</v>
@@ -2894,10 +2863,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D38" s="8">
         <v>45712</v>
@@ -2908,10 +2877,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C39" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>185</v>
       </c>
       <c r="D39" s="8">
         <v>45713</v>
@@ -2922,10 +2891,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D40" s="8">
         <v>45715</v>
@@ -2939,7 +2908,7 @@
         <v>32</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D41" s="8">
         <v>45716</v>
@@ -2953,7 +2922,7 @@
         <v>32</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D42" s="8">
         <v>45717</v>
@@ -2964,49 +2933,55 @@
         <v>42</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D43" s="8">
         <v>45719</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="16">
+    <row r="44" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A44" s="15">
         <v>43</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C44" s="14" t="s">
         <v>187</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>189</v>
       </c>
       <c r="D44" s="8">
         <v>45720</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="16">
+    <row r="45" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A45" s="15">
         <v>44</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="16">
+      <c r="C45" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="D45" s="8">
+        <v>45721</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A46" s="15">
         <v>45</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="12" t="s">
-        <v>214</v>
+      <c r="C46" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="D46" s="8">
+        <v>45722</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
@@ -3014,10 +2989,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+      <c r="D47" s="8">
+        <v>45723</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
@@ -3025,10 +3003,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3036,10 +3014,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3047,10 +3025,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3058,10 +3036,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3069,10 +3047,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3080,10 +3058,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C53" s="12" t="s">
         <v>193</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3102,10 +3080,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3113,10 +3091,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="C56" s="12" t="s">
         <v>196</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3127,7 +3105,7 @@
         <v>34</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3138,7 +3116,7 @@
         <v>36</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3149,7 +3127,7 @@
         <v>36</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3157,10 +3135,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3168,10 +3146,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C61" s="12" t="s">
         <v>201</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3179,10 +3157,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3193,7 +3171,7 @@
         <v>37</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3204,7 +3182,7 @@
         <v>37</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3212,10 +3190,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3223,10 +3201,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C66" s="12" t="s">
         <v>206</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3237,7 +3215,7 @@
         <v>38</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3248,7 +3226,7 @@
         <v>38</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3256,10 +3234,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3267,10 +3245,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -3278,10 +3256,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="C71" s="12" t="s">
         <v>211</v>
-      </c>
-      <c r="C71" s="12" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Leetcode: 1365 solution added. Syllabus: updated till date. Mini Project: registration list updated
</commit_message>
<xml_diff>
--- a/Syllabus.xlsx
+++ b/Syllabus.xlsx
@@ -1370,7 +1370,7 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2018,13 +2018,13 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="16">
+      <c r="A46" s="15">
         <v>46</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="6" t="s">
         <v>106</v>
       </c>
       <c r="D46" s="8">
@@ -2032,28 +2032,34 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="16">
+      <c r="A47" s="15">
         <v>47</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="6" t="s">
         <v>106</v>
       </c>
+      <c r="D47" s="8">
+        <v>45724</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="16">
+      <c r="A48" s="15">
         <v>48</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="17" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="8">
+        <v>45726</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
         <v>49</v>
       </c>
@@ -2063,8 +2069,11 @@
       <c r="C49" s="4" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="8">
+        <v>45727</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
         <v>50</v>
       </c>
@@ -2075,7 +2084,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
         <v>51</v>
       </c>
@@ -2086,7 +2095,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
         <v>52</v>
       </c>
@@ -2097,7 +2106,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
         <v>53</v>
       </c>
@@ -2108,7 +2117,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
         <v>54</v>
       </c>
@@ -2119,7 +2128,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
         <v>55</v>
       </c>
@@ -2130,7 +2139,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="16">
         <v>56</v>
       </c>
@@ -2141,7 +2150,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="16">
         <v>57</v>
       </c>
@@ -2152,7 +2161,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="16">
         <v>58</v>
       </c>
@@ -2163,7 +2172,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="16">
         <v>59</v>
       </c>
@@ -2174,7 +2183,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="16">
         <v>60</v>
       </c>
@@ -2185,7 +2194,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="16">
         <v>61</v>
       </c>
@@ -2196,7 +2205,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="16">
         <v>62</v>
       </c>
@@ -2207,7 +2216,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A63" s="16">
         <v>63</v>
       </c>
@@ -2218,7 +2227,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A64" s="16">
         <v>64</v>
       </c>
@@ -2328,7 +2337,7 @@
   <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46:D47"/>
+      <selection activeCell="D49" sqref="D49:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2984,43 +2993,49 @@
         <v>45722</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="16">
+    <row r="47" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A47" s="15">
         <v>46</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="14" t="s">
         <v>153</v>
       </c>
       <c r="D47" s="8">
         <v>45723</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="16">
+    <row r="48" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A48" s="15">
         <v>47</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B48" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C48" s="14" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="16">
+      <c r="D48" s="8">
+        <v>45724</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A49" s="15">
         <v>48</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="14" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D49" s="8">
+        <v>45726</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" s="16">
         <v>49</v>
       </c>
@@ -3030,8 +3045,11 @@
       <c r="C50" s="12" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D50" s="8">
+        <v>45727</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51" s="16">
         <v>50</v>
       </c>
@@ -3042,7 +3060,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52" s="16">
         <v>51</v>
       </c>
@@ -3053,7 +3071,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53" s="16">
         <v>52</v>
       </c>
@@ -3064,7 +3082,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" s="16">
         <v>53</v>
       </c>
@@ -3075,7 +3093,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" s="16">
         <v>54</v>
       </c>
@@ -3086,7 +3104,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="16">
         <v>55</v>
       </c>
@@ -3097,7 +3115,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="16">
         <v>56</v>
       </c>
@@ -3108,7 +3126,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" s="16">
         <v>57</v>
       </c>
@@ -3119,7 +3137,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A59" s="16">
         <v>58</v>
       </c>
@@ -3130,7 +3148,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="16">
         <v>59</v>
       </c>
@@ -3141,7 +3159,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="16">
         <v>60</v>
       </c>
@@ -3152,7 +3170,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" s="16">
         <v>61</v>
       </c>
@@ -3163,7 +3181,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="16">
         <v>62</v>
       </c>
@@ -3174,7 +3192,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" s="16">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Graph algorithm: Dijkstra Algo added
</commit_message>
<xml_diff>
--- a/Syllabus.xlsx
+++ b/Syllabus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Java_FSD" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="217">
   <si>
     <t>Topic</t>
   </si>
@@ -436,161 +436,10 @@
     <t>Introduction to Mockito, Creating Mocks, Stubbing Methods, Verifying Interactions</t>
   </si>
   <si>
-    <t>Testing in Spring Applications</t>
-  </si>
-  <si>
-    <t>Writing Unit Tests for Spring Layers</t>
-  </si>
-  <si>
-    <t>Service Layer Tests, Repository Layer Tests, Controller Layer Tests with MockMVC</t>
-  </si>
-  <si>
-    <t>Advanced Testing and Best Practices</t>
-  </si>
-  <si>
-    <t>Test Coverage, Writing Clean Tests, Debugging Failing Tests, Continuous Testing with CI/CD</t>
-  </si>
-  <si>
     <t>Introduction and Usage of useEffect</t>
   </si>
   <si>
     <t>Creating Custom Hooks, React Memo, and React.memo</t>
-  </si>
-  <si>
-    <r>
-      <t>Query Operators ($and</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>$or</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>$gt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>$lt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>$in</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>), Regular Expressions, and Text Search</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Aggregation Pipeline, $match</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>$group</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>$project</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, Sorting, and Limiting</t>
-    </r>
   </si>
   <si>
     <r>
@@ -711,47 +560,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Spring Testing Annotations (@RunWith</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>@SpringBootTest</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">), Mocking Beans with </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>@MockBean</t>
-    </r>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -905,9 +713,6 @@
     <t>Analyzing Space-Time Trade-offs</t>
   </si>
   <si>
-    <t>Concept, Greedy vs. DP</t>
-  </si>
-  <si>
     <t>Problems (Activity Selection, Huffman Coding)</t>
   </si>
   <si>
@@ -926,12 +731,6 @@
     <t>Minimum Spanning Tree (Kruskal, Prim)</t>
   </si>
   <si>
-    <t>Graph Algorithms (Hands-on)</t>
-  </si>
-  <si>
-    <t>Implementing Graph Algorithms</t>
-  </si>
-  <si>
     <t>Problem Solving</t>
   </si>
   <si>
@@ -969,13 +768,28 @@
   </si>
   <si>
     <t>Creating APIs, @RestController, Spring Boot DevTools</t>
+  </si>
+  <si>
+    <t>ALPHA - WORKSHOP</t>
+  </si>
+  <si>
+    <t>BETA - WORKSHOP</t>
+  </si>
+  <si>
+    <t>Query Operators ($and, $or, $gt, $lt, $in), Regular Expressions, and Text Search</t>
+  </si>
+  <si>
+    <t>Last Lecture Hour</t>
+  </si>
+  <si>
+    <t>Aggregation Pipeline, $match, $group, $project, Sorting, and Limiting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1036,8 +850,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1065,6 +886,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1075,13 +901,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1122,9 +949,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1136,8 +960,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="9" fillId="6" borderId="0" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
+    <cellStyle name="Accent2" xfId="6" builtinId="33"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
@@ -1358,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView topLeftCell="A61" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1368,7 +1196,7 @@
     <col min="2" max="2" width="38.5546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="73.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
@@ -1383,7 +1211,7 @@
         <v>40</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1486,7 +1314,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>2</v>
@@ -1575,10 +1403,10 @@
       <c r="A15" s="9">
         <v>15</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="16" t="s">
         <v>55</v>
       </c>
       <c r="D15" s="8">
@@ -1589,25 +1417,25 @@
       <c r="A16" s="9">
         <v>16</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>216</v>
+      <c r="B16" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>205</v>
       </c>
       <c r="D16" s="10">
         <v>45684</v>
       </c>
-      <c r="E16" s="18"/>
+      <c r="E16" s="17"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>17</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>57</v>
       </c>
       <c r="D17" s="8">
@@ -1618,10 +1446,10 @@
       <c r="A18" s="15">
         <v>18</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>59</v>
       </c>
       <c r="D18" s="8">
@@ -1632,10 +1460,10 @@
       <c r="A19" s="15">
         <v>19</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="16" t="s">
         <v>61</v>
       </c>
       <c r="D19" s="8">
@@ -1646,10 +1474,10 @@
       <c r="A20" s="15">
         <v>20</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>63</v>
       </c>
       <c r="D20" s="8">
@@ -1660,10 +1488,10 @@
       <c r="A21" s="15">
         <v>21</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="16" t="s">
         <v>65</v>
       </c>
       <c r="D21" s="8">
@@ -1674,11 +1502,11 @@
       <c r="A22" s="15">
         <v>22</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>217</v>
+      <c r="C22" s="16" t="s">
+        <v>206</v>
       </c>
       <c r="D22" s="8">
         <v>45691</v>
@@ -1688,10 +1516,10 @@
       <c r="A23" s="15">
         <v>23</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="16" t="s">
         <v>68</v>
       </c>
       <c r="D23" s="8">
@@ -1702,11 +1530,11 @@
       <c r="A24" s="15">
         <v>24</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>143</v>
+      <c r="B24" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>138</v>
       </c>
       <c r="D24" s="8">
         <v>45693</v>
@@ -1716,10 +1544,10 @@
       <c r="A25" s="15">
         <v>25</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="16" t="s">
         <v>70</v>
       </c>
       <c r="D25" s="8">
@@ -1730,11 +1558,11 @@
       <c r="A26" s="15">
         <v>26</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>219</v>
+      <c r="C26" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="D26" s="8">
         <v>45695</v>
@@ -1744,10 +1572,10 @@
       <c r="A27" s="15">
         <v>27</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="16" t="s">
         <v>73</v>
       </c>
       <c r="D27" s="8">
@@ -1758,10 +1586,10 @@
       <c r="A28" s="15">
         <v>28</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="16" t="s">
         <v>75</v>
       </c>
       <c r="D28" s="8">
@@ -1772,10 +1600,10 @@
       <c r="A29" s="15">
         <v>29</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="16" t="s">
         <v>77</v>
       </c>
       <c r="D29" s="8">
@@ -1786,10 +1614,10 @@
       <c r="A30" s="15">
         <v>30</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="16" t="s">
         <v>79</v>
       </c>
       <c r="D30" s="8">
@@ -1800,10 +1628,10 @@
       <c r="A31" s="15">
         <v>31</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="16" t="s">
         <v>81</v>
       </c>
       <c r="D31" s="8">
@@ -1814,11 +1642,11 @@
       <c r="A32" s="15">
         <v>32</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>144</v>
+      <c r="C32" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="D32" s="8">
         <v>45702</v>
@@ -1828,10 +1656,10 @@
       <c r="A33" s="15">
         <v>33</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="16" t="s">
         <v>84</v>
       </c>
       <c r="D33" s="8">
@@ -1842,10 +1670,10 @@
       <c r="A34" s="15">
         <v>34</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="16" t="s">
         <v>85</v>
       </c>
       <c r="D34" s="8">
@@ -1856,10 +1684,10 @@
       <c r="A35" s="15">
         <v>35</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="16" t="s">
         <v>87</v>
       </c>
       <c r="D35" s="8">
@@ -1870,10 +1698,10 @@
       <c r="A36" s="15">
         <v>36</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="16" t="s">
         <v>89</v>
       </c>
       <c r="D36" s="8">
@@ -1884,10 +1712,10 @@
       <c r="A37" s="15">
         <v>37</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="20" t="s">
         <v>91</v>
       </c>
       <c r="D37" s="8">
@@ -1898,10 +1726,10 @@
       <c r="A38" s="15">
         <v>38</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="20" t="s">
         <v>93</v>
       </c>
       <c r="D38" s="8">
@@ -1912,10 +1740,10 @@
       <c r="A39" s="15">
         <v>39</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="16" t="s">
         <v>95</v>
       </c>
       <c r="D39" s="8">
@@ -1926,10 +1754,10 @@
       <c r="A40" s="15">
         <v>40</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="16" t="s">
         <v>97</v>
       </c>
       <c r="D40" s="8">
@@ -1940,10 +1768,10 @@
       <c r="A41" s="15">
         <v>41</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="16" t="s">
         <v>99</v>
       </c>
       <c r="D41" s="8">
@@ -1954,10 +1782,10 @@
       <c r="A42" s="15">
         <v>42</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="16" t="s">
         <v>101</v>
       </c>
       <c r="D42" s="8">
@@ -1968,11 +1796,11 @@
       <c r="A43" s="15">
         <v>43</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>220</v>
+      <c r="C43" s="16" t="s">
+        <v>209</v>
       </c>
       <c r="D43" s="8">
         <v>45720</v>
@@ -1982,10 +1810,10 @@
       <c r="A44" s="15">
         <v>44</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="16" t="s">
         <v>104</v>
       </c>
       <c r="D44" s="8">
@@ -1996,11 +1824,11 @@
       <c r="A45" s="15">
         <v>45</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C45" s="17" t="s">
-        <v>221</v>
+      <c r="C45" s="16" t="s">
+        <v>210</v>
       </c>
       <c r="D45" s="8">
         <v>45722</v>
@@ -2038,294 +1866,323 @@
       <c r="A48" s="15">
         <v>48</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="16" t="s">
         <v>108</v>
       </c>
       <c r="D48" s="8">
         <v>45726</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <v>49</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="C49" s="17" t="s">
-        <v>222</v>
+      <c r="C49" s="16" t="s">
+        <v>211</v>
       </c>
       <c r="D49" s="8">
         <v>45727</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <v>50</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C50" s="16" t="s">
         <v>111</v>
       </c>
       <c r="D50" s="8">
         <v>45728</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <v>51</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="C51" s="16" t="s">
         <v>113</v>
       </c>
       <c r="D51" s="8">
         <v>45729</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <v>52</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C52" s="16" t="s">
         <v>115</v>
       </c>
       <c r="D52" s="8">
         <v>45731</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="16">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="15">
         <v>53</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="6" t="s">
         <v>116</v>
       </c>
       <c r="D53" s="8">
         <v>45733</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="16">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="15">
         <v>54</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="6" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="16">
+      <c r="D54" s="8">
+        <v>45734</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="15">
         <v>55</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="16">
+      <c r="B55" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="D55" s="8">
+        <v>45735</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="15">
         <v>56</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="16">
+      <c r="B56" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D56" s="8">
+        <v>45736</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A57" s="15">
         <v>57</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="16">
+      <c r="B57" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D57" s="8">
+        <v>45737</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="15">
         <v>58</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="16">
+      <c r="B58" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D58" s="8">
+        <v>45738</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A59" s="15">
         <v>59</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="16">
+      <c r="B59" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="D59" s="8">
+        <v>45740</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="15">
         <v>60</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="16">
+      <c r="B60" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="D60" s="8">
+        <v>45741</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A61" s="15">
         <v>61</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="16">
+      <c r="B61" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D61" s="8">
+        <v>45742</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A62" s="15">
         <v>62</v>
       </c>
-      <c r="B62" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A63" s="16">
+      <c r="B62" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62" s="8">
+        <v>45743</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A63" s="15">
         <v>63</v>
       </c>
-      <c r="B63" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A64" s="16">
+      <c r="B63" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D63" s="8">
+        <v>45744</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A64" s="15">
         <v>64</v>
       </c>
-      <c r="B64" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A65" s="16">
+      <c r="B64" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="D64" s="8">
+        <v>45745</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A65" s="15">
         <v>65</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A66" s="16">
+        <v>140</v>
+      </c>
+      <c r="D65" s="8">
+        <v>45749</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="15">
         <v>66</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A67" s="16">
+        <v>141</v>
+      </c>
+      <c r="D66" s="8">
+        <v>45750</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="15">
         <v>67</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="16">
-        <v>68</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="16">
-        <v>69</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C69" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A70" s="16">
-        <v>70</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="16">
-        <v>71</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A72" s="16">
-        <v>72</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>142</v>
-      </c>
+      <c r="D67" s="21">
+        <v>45751</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="17"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="17"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="17"/>
+      <c r="D69" s="17"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="17"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="17"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="17"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2335,10 +2192,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2347,7 +2204,8 @@
     <col min="2" max="2" width="40.109375" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63.88671875" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="11"/>
+    <col min="5" max="5" width="15.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
@@ -2358,10 +2216,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
@@ -2372,7 +2230,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D2" s="8">
         <v>45659</v>
@@ -2386,7 +2244,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="D3" s="8">
         <v>45660</v>
@@ -2400,7 +2258,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="D4" s="8">
         <v>45661</v>
@@ -2439,10 +2297,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="D7" s="8">
         <v>45665</v>
@@ -2456,7 +2314,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D8" s="8">
         <v>45666</v>
@@ -2467,10 +2325,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D9" s="8">
         <v>45667</v>
@@ -2481,10 +2339,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D10" s="8">
         <v>45668</v>
@@ -2509,10 +2367,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D12" s="8">
         <v>45678</v>
@@ -2523,10 +2381,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D13" s="8">
         <v>45679</v>
@@ -2537,10 +2395,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="D14" s="8">
         <v>45680</v>
@@ -2565,10 +2423,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D16" s="8">
         <v>45682</v>
@@ -2579,10 +2437,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="D17" s="10">
         <v>45684</v>
@@ -2593,10 +2451,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D18" s="8">
         <v>45685</v>
@@ -2621,10 +2479,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="D20" s="8">
         <v>45687</v>
@@ -2634,10 +2492,10 @@
       <c r="A21" s="15">
         <v>20</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="8">
@@ -2649,10 +2507,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D22" s="8">
         <v>45689</v>
@@ -2663,10 +2521,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D23" s="8">
         <v>45691</v>
@@ -2691,7 +2549,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>23</v>
@@ -2705,10 +2563,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="D26" s="8">
         <v>45694</v>
@@ -2733,10 +2591,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D28" s="8">
         <v>45696</v>
@@ -2747,10 +2605,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D29" s="8">
         <v>45698</v>
@@ -2775,10 +2633,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="D31" s="8">
         <v>45700</v>
@@ -2789,10 +2647,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D32" s="8">
         <v>45701</v>
@@ -2806,7 +2664,7 @@
         <v>26</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="D33" s="8">
         <v>45702</v>
@@ -2831,10 +2689,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D35" s="8">
         <v>45705</v>
@@ -2845,10 +2703,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D36" s="8">
         <v>45706</v>
@@ -2861,7 +2719,7 @@
       <c r="B37" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="19" t="s">
         <v>31</v>
       </c>
       <c r="D37" s="8">
@@ -2872,11 +2730,11 @@
       <c r="A38" s="15">
         <v>37</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>181</v>
+      <c r="B38" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>173</v>
       </c>
       <c r="D38" s="8">
         <v>45712</v>
@@ -2887,10 +2745,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D39" s="8">
         <v>45713</v>
@@ -2901,10 +2759,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="D40" s="8">
         <v>45715</v>
@@ -2918,7 +2776,7 @@
         <v>32</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D41" s="8">
         <v>45716</v>
@@ -2932,7 +2790,7 @@
         <v>32</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D42" s="8">
         <v>45717</v>
@@ -2943,10 +2801,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D43" s="8">
         <v>45719</v>
@@ -2957,10 +2815,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D44" s="8">
         <v>45720</v>
@@ -2974,7 +2832,7 @@
         <v>33</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D45" s="8">
         <v>45721</v>
@@ -2988,7 +2846,7 @@
         <v>33</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D46" s="8">
         <v>45722</v>
@@ -2999,10 +2857,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D47" s="8">
         <v>45723</v>
@@ -3013,10 +2871,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D48" s="8">
         <v>45724</v>
@@ -3027,10 +2885,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="D49" s="8">
         <v>45726</v>
@@ -3041,10 +2899,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="D50" s="8">
         <v>45727</v>
@@ -3055,10 +2913,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="D51" s="8">
         <v>45728</v>
@@ -3069,10 +2927,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D52" s="8">
         <v>45729</v>
@@ -3083,260 +2941,272 @@
         <v>52</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D53" s="8">
         <v>45731</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A54" s="16">
+    <row r="54" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A54" s="15">
         <v>53</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B54" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="14" t="s">
         <v>35</v>
       </c>
       <c r="D54" s="8">
         <v>45733</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A55" s="16">
+    <row r="55" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A55" s="15">
         <v>54</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55" s="8">
+        <v>45734</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A56" s="15">
+        <v>55</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="D56" s="8">
+        <v>45735</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A57" s="15">
+        <v>56</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="D57" s="8">
+        <v>45736</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A58" s="15">
+        <v>57</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="D58" s="8">
+        <v>45737</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A59" s="15">
+        <v>58</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="D59" s="8">
+        <v>45738</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A60" s="15">
+        <v>59</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D60" s="8">
+        <v>45740</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A61" s="15">
+        <v>60</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D61" s="8">
+        <v>45741</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A62" s="15">
+        <v>61</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="D62" s="8">
+        <v>45742</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A63" s="15">
+        <v>62</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="D63" s="8">
+        <v>45743</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A64" s="15">
+        <v>63</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="D64" s="8">
+        <v>45744</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A65" s="15">
+        <v>64</v>
+      </c>
+      <c r="B65" s="14" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A56" s="16">
-        <v>55</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="C56" s="12" t="s">
+      <c r="C65" s="14" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A57" s="16">
-        <v>56</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A58" s="16">
-        <v>57</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C58" s="12" t="s">
+      <c r="D65" s="8">
+        <v>45745</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A66" s="15">
+        <v>65</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="C66" s="14" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A59" s="16">
-        <v>58</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C59" s="12" t="s">
+      <c r="D66" s="8">
+        <v>45749</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A67" s="15">
+        <v>66</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C67" s="14" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A60" s="16">
-        <v>59</v>
-      </c>
-      <c r="B60" s="12" t="s">
+      <c r="D67" s="8">
+        <v>45750</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A68" s="15">
+        <v>67</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C68" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="C60" s="12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A61" s="16">
-        <v>60</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A62" s="16">
-        <v>61</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A63" s="16">
-        <v>62</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A64" s="16">
-        <v>63</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C64" s="12" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A65" s="16">
-        <v>64</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A66" s="16">
-        <v>65</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A67" s="16">
-        <v>66</v>
-      </c>
-      <c r="B67" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A68" s="16">
-        <v>67</v>
-      </c>
-      <c r="B68" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A69" s="16">
-        <v>68</v>
-      </c>
-      <c r="B69" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="C69" s="12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A70" s="16">
-        <v>69</v>
-      </c>
-      <c r="B70" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="C70" s="12" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A71" s="16">
-        <v>70</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="C71" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D68" s="21">
+        <v>45751</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A69" s="12"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+    </row>
+    <row r="70" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A70" s="12"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
+    </row>
+    <row r="71" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A71" s="12"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+    </row>
+    <row r="72" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A72" s="12"/>
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
     </row>
-    <row r="73" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A73" s="12"/>
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
     </row>
-    <row r="74" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A74" s="12"/>
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
     </row>
-    <row r="75" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A75" s="12"/>
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
     </row>
-    <row r="76" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A76" s="12"/>
       <c r="B76" s="12"/>
       <c r="C76" s="12"/>
     </row>
-    <row r="77" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A77" s="12"/>
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
-    </row>
-    <row r="78" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A78" s="12"/>
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-    </row>
-    <row r="79" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A79" s="12"/>
-      <c r="B79" s="12"/>
-      <c r="C79" s="12"/>
-    </row>
-    <row r="80" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A80" s="12"/>
-      <c r="B80" s="12"/>
-      <c r="C80" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>